<commit_message>
Minimize pjm5bus test case for Jumper modeling
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_jumper.xlsx
+++ b/ams/cases/5bus/pjm5bus_jumper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728107F2-4D3D-FA49-9927-73D8ECB51EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F772A88-6FF8-534E-B852-B823E15F3B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -23,15 +23,6 @@
     <sheet name="Area" sheetId="6" r:id="rId8"/>
     <sheet name="Zone" sheetId="10" r:id="rId9"/>
     <sheet name="GCost" sheetId="11" r:id="rId10"/>
-    <sheet name="SRCost" sheetId="18" r:id="rId11"/>
-    <sheet name="SFRCost" sheetId="16" r:id="rId12"/>
-    <sheet name="DCost" sheetId="22" r:id="rId13"/>
-    <sheet name="NSRCost" sheetId="20" r:id="rId14"/>
-    <sheet name="EDTSlot" sheetId="12" r:id="rId15"/>
-    <sheet name="UCTSlot" sheetId="13" r:id="rId16"/>
-    <sheet name="SFR" sheetId="15" r:id="rId17"/>
-    <sheet name="SR" sheetId="17" r:id="rId18"/>
-    <sheet name="NSR" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="114">
   <si>
     <t>idx</t>
   </si>
@@ -194,12 +185,6 @@
     <t>ZONE_1</t>
   </si>
   <si>
-    <t>ZONE1</t>
-  </si>
-  <si>
-    <t>ZONE2</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -266,63 +251,6 @@
     <t>Slack_4</t>
   </si>
   <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>EDT1</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>EDT2</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>EDT3</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>EDT4</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>EDT5</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>EDT6</t>
-  </si>
-  <si>
-    <t>UCT1</t>
-  </si>
-  <si>
-    <t>UCT2</t>
-  </si>
-  <si>
-    <t>UCT3</t>
-  </si>
-  <si>
-    <t>UCT4</t>
-  </si>
-  <si>
-    <t>UCT5</t>
-  </si>
-  <si>
-    <t>UCT6</t>
-  </si>
-  <si>
     <t>PQ_1</t>
   </si>
   <si>
@@ -332,90 +260,9 @@
     <t>PQ_3</t>
   </si>
   <si>
-    <t>demand</t>
-  </si>
-  <si>
-    <t>SR1</t>
-  </si>
-  <si>
-    <t>SR2</t>
-  </si>
-  <si>
-    <t>csr</t>
-  </si>
-  <si>
-    <t>SRC_1</t>
-  </si>
-  <si>
-    <t>SRC_2</t>
-  </si>
-  <si>
-    <t>SRC_3</t>
-  </si>
-  <si>
-    <t>SRC_4</t>
-  </si>
-  <si>
-    <t>cru</t>
-  </si>
-  <si>
-    <t>crd</t>
-  </si>
-  <si>
-    <t>SFRC_1</t>
-  </si>
-  <si>
-    <t>SFRC_2</t>
-  </si>
-  <si>
-    <t>SFRC_3</t>
-  </si>
-  <si>
-    <t>SFRC_4</t>
-  </si>
-  <si>
-    <t>NSR1</t>
-  </si>
-  <si>
-    <t>NSR2</t>
-  </si>
-  <si>
-    <t>cnsr</t>
-  </si>
-  <si>
-    <t>NSRC_1</t>
-  </si>
-  <si>
-    <t>NSRC_2</t>
-  </si>
-  <si>
-    <t>NSRC_3</t>
-  </si>
-  <si>
-    <t>NSRC_4</t>
-  </si>
-  <si>
     <t>ZONE_2</t>
   </si>
   <si>
-    <t>0.793, 0</t>
-  </si>
-  <si>
-    <t>0.756, 0</t>
-  </si>
-  <si>
-    <t>0.723, 0</t>
-  </si>
-  <si>
-    <t>0.708, 0</t>
-  </si>
-  <si>
-    <t>0.7, 0</t>
-  </si>
-  <si>
-    <t>0.706, 0</t>
-  </si>
-  <si>
     <t>field</t>
   </si>
   <si>
@@ -431,39 +278,15 @@
     <t>About</t>
   </si>
   <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>StaticGen</t>
-  </si>
-  <si>
-    <t>Minimum on/off time of generators were made up</t>
-  </si>
-  <si>
     <t>PJM 5-bus test case</t>
   </si>
   <si>
-    <t>Load factor in EDTSlot and UCTSlot sourced from PJM 5-minutes load on August 30, 2023</t>
-  </si>
-  <si>
     <t>td1</t>
   </si>
   <si>
     <t>td2</t>
   </si>
   <si>
-    <t>du</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>SFR1</t>
-  </si>
-  <si>
-    <t>SFR2</t>
-  </si>
-  <si>
     <t>rate_a</t>
   </si>
   <si>
@@ -473,12 +296,6 @@
     <t>rate_c</t>
   </si>
   <si>
-    <t>ug</t>
-  </si>
-  <si>
-    <t>1,1,1,1</t>
-  </si>
-  <si>
     <t>Line AB</t>
   </si>
   <si>
@@ -503,30 +320,6 @@
     <t>ctrl</t>
   </si>
   <si>
-    <t>pq</t>
-  </si>
-  <si>
-    <t>cdp</t>
-  </si>
-  <si>
-    <t>DCost_1</t>
-  </si>
-  <si>
-    <t>Dcost 1</t>
-  </si>
-  <si>
-    <t>DCost_2</t>
-  </si>
-  <si>
-    <t>Dcost 2</t>
-  </si>
-  <si>
-    <t>DCost_3</t>
-  </si>
-  <si>
-    <t>Dcost 3</t>
-  </si>
-  <si>
     <t>Line_0</t>
   </si>
   <si>
@@ -585,13 +378,19 @@
   </si>
   <si>
     <t>J1-5</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t>Test case for Jumper development and test, only include minimum data for DCOPF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,30 +428,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -666,7 +442,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -700,72 +476,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1070,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E0E47-E5E8-FA43-A027-51A5C4ADA178}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1083,16 +814,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1100,34 +831,23 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +860,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1162,22 +882,22 @@
         <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1185,16 +905,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1220,16 +940,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1255,16 +975,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1290,16 +1010,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1321,1034 +1041,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB172BE7-B3C0-A449-8F62-0781AC3DED02}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369B7ED6-0339-A34F-8D4C-28B9C408DB19}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130608C9-3E81-B940-B421-2E5FE1C369EA}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787DEB6E-5407-D64E-8FD6-1F71A62EBC04}">
-  <dimension ref="A1:E25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2777B7D7-CE5C-114E-9B38-A548A06A92E7}">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0222B4-433A-4847-9EF9-ED7322586C33}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="F2" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC4103-A416-3E41-9041-99544891E416}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2413,13 +1106,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>230</v>
@@ -2454,13 +1147,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3">
         <v>230</v>
@@ -2495,13 +1188,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4">
         <v>230</v>
@@ -2536,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2577,13 +1270,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E6">
         <v>230</v>
@@ -2614,7 +1307,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2664,8 +1357,8 @@
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>149</v>
+      <c r="L1" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2673,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2682,7 +1375,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>230</v>
@@ -2708,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2717,7 +1410,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="F3">
         <v>230</v>
@@ -2743,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2752,7 +1445,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="F4">
         <v>230</v>
@@ -2774,7 +1467,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2843,10 +1536,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -2854,21 +1547,21 @@
       <c r="U1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -2877,7 +1570,7 @@
         <v>230</v>
       </c>
       <c r="G2" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2924,13 +1617,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -2939,7 +1632,7 @@
         <v>230</v>
       </c>
       <c r="G3" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="I3">
         <v>3.2349000000000001</v>
@@ -2986,13 +1679,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -3001,7 +1694,7 @@
         <v>230</v>
       </c>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="I4">
         <v>4.6650999999999998</v>
@@ -3111,11 +1804,11 @@
       <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>132</v>
+      <c r="R1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -3132,13 +1825,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -3147,7 +1840,7 @@
         <v>230</v>
       </c>
       <c r="G2" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3193,8 +1886,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3236,19 +1929,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3308,13 +2001,13 @@
         <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>36</v>
@@ -3355,19 +2048,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -3429,19 +2122,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -3503,19 +2196,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -3577,19 +2270,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -3651,19 +2344,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -3725,19 +2418,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -3799,19 +2492,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -3869,7 +2562,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3941,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94B98-B38A-EC46-833E-965628D04701}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3962,31 +2655,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>170</v>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>171</v>
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>